<commit_message>
Calculate Price Final Commit
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\source\repos\RASTowing\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U748986\source\repos\RASTowing\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1497CE42-2AA0-48B9-AC6D-98D0A88494E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="drivers_data" sheetId="1" r:id="rId1"/>
@@ -29,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
   <si>
-    <t>0800 031 4303</t>
-  </si>
-  <si>
     <t>2C Recovery</t>
   </si>
   <si>
@@ -211,18 +207,6 @@
     <t>Call out</t>
   </si>
   <si>
-    <t>Week-end</t>
-  </si>
-  <si>
-    <t>Night rate</t>
-  </si>
-  <si>
-    <t>Caravan/trailer</t>
-  </si>
-  <si>
-    <t>Whells dolly/ stick</t>
-  </si>
-  <si>
     <t>Jumpstart</t>
   </si>
   <si>
@@ -251,12 +235,30 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
+  <si>
+    <t>Night Rate</t>
+  </si>
+  <si>
+    <t>Whells Dolly/ Stick</t>
+  </si>
+  <si>
+    <t>Caravan/ Trailer</t>
+  </si>
+  <si>
+    <t>Wrong Fuel</t>
+  </si>
+  <si>
+    <t>0800 031 4303 / 0800 031 4303</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,7 +405,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -680,334 +682,334 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.1796875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.81640625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="E1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1016,7 +1018,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>BooleanList!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1029,45 +1031,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="9">
         <v>50</v>
@@ -1085,9 +1087,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="9">
         <v>60</v>
@@ -1105,9 +1107,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B4" s="9">
         <v>20</v>
@@ -1125,9 +1127,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="9">
         <v>20</v>
@@ -1145,9 +1147,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="9">
         <v>20</v>
@@ -1165,83 +1167,103 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9">
+        <v>20</v>
+      </c>
+      <c r="D7" s="9">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="9">
         <v>10</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C8" s="9">
         <v>10</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D8" s="9">
         <v>10</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E8" s="9">
         <v>10</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F8" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="9">
-        <v>20</v>
-      </c>
-      <c r="C8" s="9">
-        <v>20</v>
-      </c>
-      <c r="D8" s="9">
-        <v>20</v>
-      </c>
-      <c r="E8" s="9">
-        <v>20</v>
-      </c>
-      <c r="F8" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="10">
+        <v>70</v>
+      </c>
+      <c r="B9" s="9">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="9">
+        <v>20</v>
+      </c>
+      <c r="E9" s="9">
+        <v>20</v>
+      </c>
+      <c r="F9" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="10">
         <v>0.5</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C10" s="10">
         <v>0.5</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D10" s="10">
         <v>0.5</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E10" s="10">
         <v>0.5</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F10" s="10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="9">
-        <v>20</v>
-      </c>
-      <c r="C10" s="9">
-        <v>20</v>
-      </c>
-      <c r="D10" s="9">
-        <v>20</v>
-      </c>
-      <c r="E10" s="9">
-        <v>20</v>
-      </c>
-      <c r="F10" s="9">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="9">
+        <v>20</v>
+      </c>
+      <c r="C11" s="9">
+        <v>20</v>
+      </c>
+      <c r="D11" s="9">
+        <v>20</v>
+      </c>
+      <c r="E11" s="9">
+        <v>20</v>
+      </c>
+      <c r="F11" s="9">
         <v>20</v>
       </c>
     </row>
@@ -1251,7 +1273,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>TypeOfVehicles!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -1264,62 +1286,62 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32547A3-21C2-4693-B83E-5CC7D4D0BC59}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B2" s="9">
         <v>1.89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9">
         <v>1.99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B4" s="9">
         <v>2.29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B5" s="9">
         <v>2.39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B6" s="9">
         <v>2.89</v>
@@ -1331,7 +1353,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{84B1BF40-8A07-48B9-AB77-3832776988E6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>TypeOfVehicles!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -1344,62 +1366,62 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1409,28 +1431,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two rows in DriversDB
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\source\repos\RASTowing\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55384738-BBD1-45C7-BC7F-248F2E167710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4D4BE1-8BA6-4E7A-A61A-3C7D142C2299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="141">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
@@ -436,6 +436,24 @@
   </si>
   <si>
     <t>452 Purley Way, Croydon, CR0 4FE</t>
+  </si>
+  <si>
+    <t>LIO CAR REPAIRS LTD</t>
+  </si>
+  <si>
+    <t>07491 110752</t>
+  </si>
+  <si>
+    <t>101 Roosevelt Way, Dagenham, United Kingdom, RM10 8DA</t>
+  </si>
+  <si>
+    <t>ASL CAR MOTORCYCLE BREAKDOWN RECOVERY</t>
+  </si>
+  <si>
+    <t>07950 355777</t>
+  </si>
+  <si>
+    <t>56 tavistock road 165 epsom road London SM5 1QR</t>
   </si>
 </sst>
 </file>
@@ -543,7 +561,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -623,6 +641,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -908,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,6 +1879,58 @@
         <v>38</v>
       </c>
       <c r="H36" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="30" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stripe Integration & Updated Drivers List
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="156">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
@@ -256,9 +256,6 @@
   </si>
   <si>
     <t>Clarke's Recovery</t>
-  </si>
-  <si>
-    <t>07494 220220</t>
   </si>
   <si>
     <t>Fairlight Farm, Hawkswood Rd, Downham, Billericay CM11 1JZ</t>
@@ -480,6 +477,27 @@
   </si>
   <si>
     <t>Unit 6a, Excelsior Works, Rollins St, London, SE15 1EP</t>
+  </si>
+  <si>
+    <t>07853 562431</t>
+  </si>
+  <si>
+    <t>71 Belvawney Close, Chelmsford, CM1 4YR</t>
+  </si>
+  <si>
+    <t>Gregs Car Transportation</t>
+  </si>
+  <si>
+    <t>Abiola Diko Breakdown Recovery</t>
+  </si>
+  <si>
+    <t>07949 706430</t>
+  </si>
+  <si>
+    <t>3-5 Elystan Pl, London SW3 3LD, UK</t>
+  </si>
+  <si>
+    <t>07494 220220 / 07496 548725</t>
   </si>
 </sst>
 </file>
@@ -955,17 +973,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="54.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.54296875" customWidth="1"/>
     <col min="6" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
@@ -1393,10 +1411,10 @@
         <v>75</v>
       </c>
       <c r="B17" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>38</v>
@@ -1416,13 +1434,13 @@
     </row>
     <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="C18" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>38</v>
@@ -1442,13 +1460,13 @@
     </row>
     <row r="19" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="C19" s="24" t="s">
         <v>82</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>83</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>38</v>
@@ -1468,13 +1486,13 @@
     </row>
     <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="C20" s="24" t="s">
         <v>85</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>86</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>38</v>
@@ -1494,13 +1512,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="C21" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>40</v>
@@ -1520,13 +1538,13 @@
     </row>
     <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="C22" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>38</v>
@@ -1546,13 +1564,13 @@
     </row>
     <row r="23" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>94</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>95</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>38</v>
@@ -1572,13 +1590,13 @@
     </row>
     <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="C24" s="19" t="s">
         <v>97</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>98</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>38</v>
@@ -1598,13 +1616,13 @@
     </row>
     <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="C25" s="29" t="s">
         <v>100</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>101</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>38</v>
@@ -1624,13 +1642,13 @@
     </row>
     <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="C26" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>104</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>38</v>
@@ -1650,13 +1668,13 @@
     </row>
     <row r="27" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="C27" s="29" t="s">
         <v>106</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>107</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>38</v>
@@ -1676,13 +1694,13 @@
     </row>
     <row r="28" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="C28" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>110</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>40</v>
@@ -1702,13 +1720,13 @@
     </row>
     <row r="29" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="C29" s="29" t="s">
         <v>112</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>113</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>40</v>
@@ -1728,13 +1746,13 @@
     </row>
     <row r="30" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>115</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>116</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>40</v>
@@ -1754,13 +1772,13 @@
     </row>
     <row r="31" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>118</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>119</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>38</v>
@@ -1780,13 +1798,13 @@
     </row>
     <row r="32" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="C32" s="29" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>122</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>38</v>
@@ -1806,13 +1824,13 @@
     </row>
     <row r="33" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="C33" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>125</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>38</v>
@@ -1832,13 +1850,13 @@
     </row>
     <row r="34" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="C34" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>128</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>40</v>
@@ -1858,13 +1876,13 @@
     </row>
     <row r="35" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="C35" s="29" t="s">
         <v>130</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>131</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>38</v>
@@ -1884,13 +1902,13 @@
     </row>
     <row r="36" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="C36" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>134</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>38</v>
@@ -1910,13 +1928,13 @@
     </row>
     <row r="37" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="C37" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="D37" s="30" t="s">
         <v>38</v>
@@ -1936,13 +1954,13 @@
     </row>
     <row r="38" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="C38" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D38" s="30" t="s">
         <v>38</v>
@@ -1962,13 +1980,13 @@
     </row>
     <row r="39" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="C39" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="D39" s="30" t="s">
         <v>38</v>
@@ -1988,13 +2006,13 @@
     </row>
     <row r="40" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="28" t="s">
-        <v>142</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="30" t="s">
         <v>40</v>
@@ -2014,27 +2032,79 @@
     </row>
     <row r="41" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="C41" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="D41" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="30" t="s">
+      <c r="C42" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G43" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" s="30" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix error with wrong address of drivers
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="159">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
@@ -123,9 +123,6 @@
     <t>07472 640307</t>
   </si>
   <si>
-    <t>Brandon Close, Chafford Hundred, Grays, RM16 6QX</t>
-  </si>
-  <si>
     <t>VRN Recovery Service</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
   </si>
   <si>
     <t>07545 357884</t>
-  </si>
-  <si>
-    <t>Hertfordshire</t>
   </si>
   <si>
     <t>Clarke's Recovery</t>
@@ -295,9 +289,6 @@
     <t>07702 000015</t>
   </si>
   <si>
-    <t>Luton</t>
-  </si>
-  <si>
     <t>Rose &amp; Sons Recovery</t>
   </si>
   <si>
@@ -323,9 +314,6 @@
     <t>07939 824617</t>
   </si>
   <si>
-    <t>Hertfordshire SG</t>
-  </si>
-  <si>
     <t>JOSH RECOVERY SERVICE</t>
   </si>
   <si>
@@ -498,6 +486,27 @@
   </si>
   <si>
     <t>07494 220220 / 07496 548725</t>
+  </si>
+  <si>
+    <t>Grove Rd, Ware SG12 7HS</t>
+  </si>
+  <si>
+    <t>Town Hall, St Paul's Square, Bedford MK40 1RA</t>
+  </si>
+  <si>
+    <t>Brandon Close Chafford Hundred Grays RM16 6QX</t>
+  </si>
+  <si>
+    <t>20-44 Gordon St, Luton LU1 2QP</t>
+  </si>
+  <si>
+    <t>Ulez Recovery Logistics</t>
+  </si>
+  <si>
+    <t>07440 690579</t>
+  </si>
+  <si>
+    <t>111 Down Land Two Mile Ash Milton Keynes MK8 8JQ</t>
   </si>
 </sst>
 </file>
@@ -973,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1001,19 +1010,19 @@
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1021,25 +1030,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1053,19 +1062,19 @@
         <v>17</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1079,19 +1088,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1105,19 +1114,19 @@
         <v>19</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1131,19 +1140,19 @@
         <v>20</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1157,19 +1166,19 @@
         <v>21</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1183,19 +1192,19 @@
         <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1209,19 +1218,19 @@
         <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1235,19 +1244,19 @@
         <v>28</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -1258,854 +1267,880 @@
         <v>30</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>154</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>65</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>68</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>73</v>
-      </c>
       <c r="C16" s="19" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>79</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>82</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>85</v>
-      </c>
       <c r="D20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="32" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G37" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G39" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B40" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="D40" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G40" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="32" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G41" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G43" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2133,27 +2168,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="8">
         <v>50</v>
@@ -2173,7 +2208,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8">
         <v>60</v>
@@ -2193,7 +2228,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="8">
         <v>20</v>
@@ -2213,7 +2248,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8">
         <v>20</v>
@@ -2233,7 +2268,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="8">
         <v>20</v>
@@ -2253,7 +2288,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="8">
         <v>20</v>
@@ -2273,7 +2308,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="8">
         <v>10</v>
@@ -2293,7 +2328,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="8">
         <v>20</v>
@@ -2313,7 +2348,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="9">
         <v>0.5</v>
@@ -2333,7 +2368,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="8">
         <v>20</v>
@@ -2385,15 +2420,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="8">
         <v>1.89</v>
@@ -2401,7 +2436,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="8">
         <v>1.99</v>
@@ -2409,7 +2444,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="8">
         <v>2.29</v>
@@ -2417,7 +2452,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="8">
         <v>2.39</v>
@@ -2425,7 +2460,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="8">
         <v>2.89</v>
@@ -2465,47 +2500,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2526,17 +2561,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor, Job Description Template + Add Drivers
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="186">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
@@ -525,6 +525,75 @@
   </si>
   <si>
     <t>Palmers Hill Epping Essex CM16 6SD</t>
+  </si>
+  <si>
+    <t>RELIABLE RECOVERY</t>
+  </si>
+  <si>
+    <t>07538 583239</t>
+  </si>
+  <si>
+    <t>Jays247recovery</t>
+  </si>
+  <si>
+    <t>07939 584077</t>
+  </si>
+  <si>
+    <t>GB BREAKDWON RECOVERY LTD</t>
+  </si>
+  <si>
+    <t>07918 500700</t>
+  </si>
+  <si>
+    <t>AB AUTOMOTIVE MOBILE MECHANIC LTD</t>
+  </si>
+  <si>
+    <t>07843
+860337</t>
+  </si>
+  <si>
+    <t>KENT CAR BREAKERS LIMITED</t>
+  </si>
+  <si>
+    <t>07949 119978</t>
+  </si>
+  <si>
+    <t>Fairfields, Maidstone Road, Staplehurst,
+TN12 0RH</t>
+  </si>
+  <si>
+    <t>BILLINGSHURST LIMITED</t>
+  </si>
+  <si>
+    <t>01403 801403</t>
+  </si>
+  <si>
+    <t>Brooker's Rd Eagle Industrial Estate RH14
+9RZ</t>
+  </si>
+  <si>
+    <t>Craythorne House Burnside Mews TN39 3LE</t>
+  </si>
+  <si>
+    <t>118 Westfield Rd, Bletchley, Milton Keynes, MK2 2RF</t>
+  </si>
+  <si>
+    <t>11 Bishopscote Road, Luton, England, LU3
+1NX</t>
+  </si>
+  <si>
+    <t>Wellington House Auckland Close
+Bexhill East Sussex TN40 2FH</t>
+  </si>
+  <si>
+    <t>D.R.H RECOVERY</t>
+  </si>
+  <si>
+    <t>07540 183595</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Unit 2, Hoads Farm, Moat Lane, Sedlescombe, Battle, TN33 0RY</t>
   </si>
 </sst>
 </file>
@@ -632,7 +701,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -716,6 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,17 +1070,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46.26953125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.54296875" customWidth="1"/>
     <col min="6" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
@@ -2210,6 +2281,188 @@
         <v>37</v>
       </c>
       <c r="H46" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G49" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G50" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G51" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="30" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Total Lift Service Added
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="187">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
@@ -594,6 +594,9 @@
   <si>
     <t xml:space="preserve">
 Unit 2, Hoads Farm, Moat Lane, Sedlescombe, Battle, TN33 0RY</t>
+  </si>
+  <si>
+    <t>Total Lift Recovery</t>
   </si>
 </sst>
 </file>
@@ -670,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -693,6 +696,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -701,7 +715,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -786,6 +800,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1070,11 +1087,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1082,13 +1099,13 @@
     <col min="1" max="1" width="46.26953125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1102,19 +1119,22 @@
         <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1148,7 @@
         <v>37</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>39</v>
@@ -1139,8 +1159,11 @@
       <c r="H2" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1177,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>39</v>
@@ -1165,8 +1188,11 @@
       <c r="H3" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1180,7 +1206,7 @@
         <v>37</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>39</v>
@@ -1191,8 +1217,11 @@
       <c r="H4" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +1235,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>39</v>
@@ -1217,8 +1246,11 @@
       <c r="H5" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1232,7 +1264,7 @@
         <v>37</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>39</v>
@@ -1243,8 +1275,11 @@
       <c r="H6" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
@@ -1258,7 +1293,7 @@
         <v>37</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>39</v>
@@ -1269,8 +1304,11 @@
       <c r="H7" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1322,7 @@
         <v>37</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>39</v>
@@ -1295,8 +1333,11 @@
       <c r="H8" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1351,7 @@
         <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>39</v>
@@ -1321,8 +1362,11 @@
       <c r="H9" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1336,7 +1380,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>39</v>
@@ -1347,8 +1391,11 @@
       <c r="H10" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1362,7 +1409,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>39</v>
@@ -1373,8 +1420,11 @@
       <c r="H11" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1388,7 +1438,7 @@
         <v>37</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>39</v>
@@ -1399,8 +1449,11 @@
       <c r="H12" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I12" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
@@ -1417,7 +1470,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>39</v>
@@ -1425,8 +1478,11 @@
       <c r="H13" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I13" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>65</v>
       </c>
@@ -1443,7 +1499,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>39</v>
@@ -1451,8 +1507,11 @@
       <c r="H14" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I14" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>68</v>
       </c>
@@ -1466,7 +1525,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>39</v>
@@ -1477,8 +1536,11 @@
       <c r="H15" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I15" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>71</v>
       </c>
@@ -1492,7 +1554,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>39</v>
@@ -1503,8 +1565,11 @@
       <c r="H16" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I16" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>73</v>
       </c>
@@ -1518,7 +1583,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>39</v>
@@ -1529,8 +1594,11 @@
       <c r="H17" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I17" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>75</v>
       </c>
@@ -1544,7 +1612,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>39</v>
@@ -1555,8 +1623,11 @@
       <c r="H18" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="I18" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
         <v>78</v>
       </c>
@@ -1570,7 +1641,7 @@
         <v>37</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>39</v>
@@ -1581,8 +1652,11 @@
       <c r="H19" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I19" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
         <v>81</v>
       </c>
@@ -1596,7 +1670,7 @@
         <v>37</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>39</v>
@@ -1607,8 +1681,11 @@
       <c r="H20" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>84</v>
       </c>
@@ -1631,10 +1708,13 @@
         <v>39</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>86</v>
       </c>
@@ -1654,13 +1734,16 @@
         <v>37</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="I22" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>89</v>
       </c>
@@ -1677,7 +1760,7 @@
         <v>37</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>39</v>
@@ -1685,8 +1768,11 @@
       <c r="H23" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I23" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>92</v>
       </c>
@@ -1700,7 +1786,7 @@
         <v>37</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>39</v>
@@ -1711,8 +1797,11 @@
       <c r="H24" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I24" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>94</v>
       </c>
@@ -1726,7 +1815,7 @@
         <v>37</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>39</v>
@@ -1737,8 +1826,11 @@
       <c r="H25" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I25" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
         <v>97</v>
       </c>
@@ -1752,7 +1844,7 @@
         <v>37</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>39</v>
@@ -1763,8 +1855,11 @@
       <c r="H26" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I26" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>100</v>
       </c>
@@ -1778,7 +1873,7 @@
         <v>37</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>39</v>
@@ -1789,8 +1884,11 @@
       <c r="H27" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I27" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>103</v>
       </c>
@@ -1804,10 +1902,10 @@
         <v>39</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>39</v>
@@ -1815,8 +1913,11 @@
       <c r="H28" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I28" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>106</v>
       </c>
@@ -1836,13 +1937,16 @@
         <v>39</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
         <v>109</v>
       </c>
@@ -1862,13 +1966,16 @@
         <v>39</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
         <v>112</v>
       </c>
@@ -1882,7 +1989,7 @@
         <v>37</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>39</v>
@@ -1893,8 +2000,11 @@
       <c r="H31" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I31" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>115</v>
       </c>
@@ -1908,19 +2018,22 @@
         <v>37</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F32" s="30" t="s">
         <v>39</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>118</v>
       </c>
@@ -1934,7 +2047,7 @@
         <v>37</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F33" s="30" t="s">
         <v>39</v>
@@ -1945,8 +2058,11 @@
       <c r="H33" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I33" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="s">
         <v>121</v>
       </c>
@@ -1960,10 +2076,10 @@
         <v>39</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G34" s="30" t="s">
         <v>39</v>
@@ -1971,8 +2087,11 @@
       <c r="H34" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I34" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="28" t="s">
         <v>124</v>
       </c>
@@ -1986,7 +2105,7 @@
         <v>37</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>39</v>
@@ -1995,10 +2114,13 @@
         <v>39</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
         <v>127</v>
       </c>
@@ -2012,19 +2134,22 @@
         <v>37</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F36" s="30" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I36" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="32" t="s">
         <v>130</v>
       </c>
@@ -2038,7 +2163,7 @@
         <v>37</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F37" s="30" t="s">
         <v>39</v>
@@ -2049,8 +2174,11 @@
       <c r="H37" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I37" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
         <v>133</v>
       </c>
@@ -2064,7 +2192,7 @@
         <v>37</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F38" s="30" t="s">
         <v>39</v>
@@ -2075,8 +2203,11 @@
       <c r="H38" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I38" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
         <v>138</v>
       </c>
@@ -2090,19 +2221,22 @@
         <v>37</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F39" s="30" t="s">
         <v>39</v>
       </c>
       <c r="G39" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I39" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
         <v>136</v>
       </c>
@@ -2116,7 +2250,7 @@
         <v>39</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F40" s="30" t="s">
         <v>37</v>
@@ -2125,10 +2259,13 @@
         <v>37</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I40" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="32" t="s">
         <v>142</v>
       </c>
@@ -2145,7 +2282,7 @@
         <v>37</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G41" s="30" t="s">
         <v>39</v>
@@ -2153,8 +2290,11 @@
       <c r="H41" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I41" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="32" t="s">
         <v>147</v>
       </c>
@@ -2171,7 +2311,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>39</v>
@@ -2179,8 +2319,11 @@
       <c r="H42" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I42" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
         <v>148</v>
       </c>
@@ -2197,7 +2340,7 @@
         <v>37</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>39</v>
@@ -2205,8 +2348,11 @@
       <c r="H43" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I43" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>156</v>
       </c>
@@ -2223,7 +2369,7 @@
         <v>37</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G44" s="30" t="s">
         <v>39</v>
@@ -2231,8 +2377,11 @@
       <c r="H44" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I44" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="32" t="s">
         <v>159</v>
       </c>
@@ -2249,7 +2398,7 @@
         <v>37</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>39</v>
@@ -2257,8 +2406,11 @@
       <c r="H45" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I45" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="32" t="s">
         <v>162</v>
       </c>
@@ -2281,10 +2433,13 @@
         <v>37</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="32" t="s">
         <v>165</v>
       </c>
@@ -2301,7 +2456,7 @@
         <v>37</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>39</v>
@@ -2309,8 +2464,11 @@
       <c r="H47" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I47" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="32" t="s">
         <v>167</v>
       </c>
@@ -2327,7 +2485,7 @@
         <v>37</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G48" s="30" t="s">
         <v>39</v>
@@ -2335,8 +2493,11 @@
       <c r="H48" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I48" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="32" t="s">
         <v>169</v>
       </c>
@@ -2353,7 +2514,7 @@
         <v>37</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>39</v>
@@ -2361,8 +2522,11 @@
       <c r="H49" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I49" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
         <v>171</v>
       </c>
@@ -2379,7 +2543,7 @@
         <v>37</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G50" s="30" t="s">
         <v>39</v>
@@ -2387,8 +2551,11 @@
       <c r="H50" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I50" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="32" t="s">
         <v>173</v>
       </c>
@@ -2405,7 +2572,7 @@
         <v>37</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>39</v>
@@ -2413,8 +2580,11 @@
       <c r="H51" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I51" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
         <v>176</v>
       </c>
@@ -2431,7 +2601,7 @@
         <v>37</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G52" s="30" t="s">
         <v>39</v>
@@ -2439,8 +2609,11 @@
       <c r="H52" s="30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I52" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>183</v>
       </c>
@@ -2457,12 +2630,15 @@
         <v>37</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>39</v>
       </c>
       <c r="H53" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I53" s="30" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2474,10 +2650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2550,28 +2726,33 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>46</v>
+      <c r="A4" s="34" t="s">
+        <v>186</v>
       </c>
       <c r="B4" s="8">
-        <v>20</v>
+        <f>B3+40</f>
+        <v>100</v>
       </c>
       <c r="C4" s="8">
-        <v>20</v>
+        <f>C3+50</f>
+        <v>110</v>
       </c>
       <c r="D4" s="8">
-        <v>20</v>
+        <f>D3+60</f>
+        <v>130</v>
       </c>
       <c r="E4" s="8">
-        <v>20</v>
+        <f>E3+100</f>
+        <v>180</v>
       </c>
       <c r="F4" s="8">
-        <v>20</v>
+        <f>F3+140</f>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B5" s="8">
         <v>20</v>
@@ -2591,7 +2772,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="8">
         <v>20</v>
@@ -2611,7 +2792,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B7" s="8">
         <v>20</v>
@@ -2631,81 +2812,101 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B8" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C8" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E8" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F8" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E9" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F9" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.5</v>
+        <v>57</v>
+      </c>
+      <c r="B10" s="8">
+        <v>20</v>
+      </c>
+      <c r="C10" s="8">
+        <v>20</v>
+      </c>
+      <c r="D10" s="8">
+        <v>20</v>
+      </c>
+      <c r="E10" s="8">
+        <v>20</v>
+      </c>
+      <c r="F10" s="8">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B12" s="8">
         <v>20</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C12" s="8">
         <v>20</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D12" s="8">
         <v>20</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E12" s="8">
         <v>20</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="8">
         <v>20</v>
       </c>
     </row>
@@ -2714,7 +2915,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>TypeOfVehicles!$A$2:$A$6</xm:f>

</xml_diff>

<commit_message>
Update drivers and adjust labeling in the main.html
</commit_message>
<xml_diff>
--- a/static/DriversDB.xlsx
+++ b/static/DriversDB.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="196">
   <si>
     <t xml:space="preserve">Sams Breakdown Recovery </t>
   </si>
@@ -597,6 +597,33 @@
   </si>
   <si>
     <t>Total Lift Recovery</t>
+  </si>
+  <si>
+    <t>GMC BREAKDOWN RECOVERY LTD</t>
+  </si>
+  <si>
+    <t>07838 666656</t>
+  </si>
+  <si>
+    <t>39 Chequers Way, Woodley, Reading, England, RG5 3EH</t>
+  </si>
+  <si>
+    <t>ROAD 2 RECOVERY</t>
+  </si>
+  <si>
+    <t>07479 032059</t>
+  </si>
+  <si>
+    <t>27 Hale Ln, Otford, Sevenoaks TN14 5NP</t>
+  </si>
+  <si>
+    <t>247 TYRE MOBILE LTD</t>
+  </si>
+  <si>
+    <t>020 3488 6465</t>
+  </si>
+  <si>
+    <t>71-75 Shelton Street, Covent Garden WC2H 9JQ</t>
   </si>
 </sst>
 </file>
@@ -1087,11 +1114,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2639,6 +2666,93 @@
         <v>39</v>
       </c>
       <c r="I53" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I55" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="G56" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="I56" s="30" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>